<commit_message>
updated MOM reports with Action plan
</commit_message>
<xml_diff>
--- a/MOM Reports/Action plans data.xlsx
+++ b/MOM Reports/Action plans data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>S. No</t>
   </si>
@@ -43,6 +43,18 @@
   </si>
   <si>
     <t>Open</t>
+  </si>
+  <si>
+    <t>Extend the project scope to the team of 5</t>
+  </si>
+  <si>
+    <t>Vikas, Sai Krishna, Revanth, Siri, Sai Teja</t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>Complete team deliverable 1 documents</t>
   </si>
 </sst>
 </file>
@@ -91,17 +103,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="7">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -127,7 +147,20 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -143,14 +176,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E2" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:E2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E4" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+  <autoFilter ref="A1:E4"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="S. No"/>
-    <tableColumn id="2" name="Action items"/>
-    <tableColumn id="3" name="Owners"/>
-    <tableColumn id="4" name="Deadline" dataDxfId="1"/>
-    <tableColumn id="5" name="Status"/>
+    <tableColumn id="1" name="S. No" dataDxfId="6"/>
+    <tableColumn id="2" name="Action items" dataDxfId="5"/>
+    <tableColumn id="3" name="Owners" dataDxfId="4"/>
+    <tableColumn id="4" name="Deadline" dataDxfId="3"/>
+    <tableColumn id="5" name="Status" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -419,21 +452,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="43.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="37" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" customWidth="1"/>
     <col min="5" max="5" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -450,20 +483,54 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="3">
+        <v>43349</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="3">
+        <v>43355</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D4" s="3">
         <v>43361</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E4" s="2" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>